<commit_message>
Fix export payment history agency
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Agency.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/Statement_of_Receivable-Agency.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="0" windowWidth="14383" windowHeight="7723"/>
+    <workbookView xWindow="9330" yWindow="0" windowWidth="14385" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="AGENCY (2)" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>TOTAL</t>
   </si>
@@ -661,6 +661,9 @@
   </si>
   <si>
     <t>{Debit_Ending}</t>
+  </si>
+  <si>
+    <t>{Credit_Ending}</t>
   </si>
 </sst>
 </file>
@@ -1043,6 +1046,36 @@
     <xf numFmtId="44" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1079,38 +1112,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="7" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1465,155 +1468,155 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomRight" activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3828125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.53515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="13.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.15234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.15234375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.84375" style="1"/>
+    <col min="19" max="19" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.140625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
     </row>
     <row r="2" spans="2:22">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="2:22" ht="15" customHeight="1">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="55" t="s">
+      <c r="O3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="50" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="51" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="51" t="s">
+      <c r="V3" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="49" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
       <c r="O4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1632,8 +1635,8 @@
       <c r="T4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
     </row>
     <row r="5" spans="2:22" s="12" customFormat="1">
       <c r="B5" s="13">
@@ -1717,7 +1720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:22" s="17" customFormat="1" ht="12.9">
+    <row r="6" spans="2:22" s="17" customFormat="1" ht="12.75">
       <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
@@ -1764,7 +1767,9 @@
       <c r="S6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="25"/>
+      <c r="T6" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="U6" s="21" t="s">
         <v>35</v>
       </c>
@@ -1772,7 +1777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:22" s="34" customFormat="1" ht="12.9">
+    <row r="7" spans="2:22" s="34" customFormat="1" ht="12.75">
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="27"/>
@@ -1786,7 +1791,7 @@
       <c r="L7" s="28"/>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
-      <c r="O7" s="58" t="s">
+      <c r="O7" s="36" t="s">
         <v>40</v>
       </c>
       <c r="P7" s="35"/>
@@ -1846,13 +1851,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:R3"/>
     <mergeCell ref="B1:U1"/>
     <mergeCell ref="B2:U2"/>
     <mergeCell ref="B3:B4"/>
@@ -1865,6 +1863,13 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:R3"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:G4">
     <cfRule type="duplicateValues" dxfId="5" priority="6" stopIfTrue="1"/>

</xml_diff>